<commit_message>
fix typos in sample arc, update playground.fsx
</commit_message>
<xml_diff>
--- a/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
+++ b/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E4B218-8A0F-43E9-A5A2-555450ABA28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CAEF62-9BD3-4BBD-94F9-73627ED0C392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="630" windowWidth="15045" windowHeight="14325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="3380" windowWidth="18000" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_assay" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>C1_measured</t>
-  </si>
-  <si>
     <t>MSFragger</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>http://purl.obolibrary.org/obo/MS_1003014</t>
   </si>
   <si>
-    <t>C2_measured</t>
-  </si>
-  <si>
     <t>Co1_measured</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>sampleOutCold.txt</t>
+  </si>
+  <si>
+    <t>CC1_measured</t>
+  </si>
+  <si>
+    <t>CC2_measured</t>
   </si>
 </sst>
 </file>
@@ -560,14 +560,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -575,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -599,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -607,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -615,12 +615,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -628,62 +628,62 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -699,25 +699,25 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.81640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.81640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="37.81640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -752,106 +752,106 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="K7" t="s">
         <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update querymodel test objects
</commit_message>
<xml_diff>
--- a/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
+++ b/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CAEF62-9BD3-4BBD-94F9-73627ED0C392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E45E72-58B5-4CBD-AA47-1B6EB63DD811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="3380" windowWidth="18000" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_assay" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Assay Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>Source Name</t>
-  </si>
-  <si>
     <t>Parameter [acquisition software]</t>
   </si>
   <si>
@@ -129,9 +126,6 @@
     <t>Term Accession Number (MS:1001457)</t>
   </si>
   <si>
-    <t>Sample Name</t>
-  </si>
-  <si>
     <t>MSFragger</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>CC2_measured</t>
+  </si>
+  <si>
+    <t>Input [Raw Data File]</t>
+  </si>
+  <si>
+    <t>Output [Derived Data File]</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}" name="annotationTableNiceZebra52" displayName="annotationTableNiceZebra52" ref="A1:K7" totalsRowShown="0">
   <autoFilter ref="A1:K7" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{35BBF576-4739-4AFC-8D38-3FE476BCD5E1}" name="Source Name"/>
+    <tableColumn id="1" xr3:uid="{35BBF576-4739-4AFC-8D38-3FE476BCD5E1}" name="Input [Raw Data File]"/>
     <tableColumn id="3" xr3:uid="{252EA98B-77DC-4AB6-BE58-C1B81480FE69}" name="Parameter [acquisition software]" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{283FEE7D-D234-44B9-9AD8-16CD15CAC244}" name="Term Source REF (MS:1001455)" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{B489FA80-D06A-4FA4-B75B-39F1B7AB9163}" name="Term Accession Number (MS:1001455)" dataDxfId="6"/>
@@ -253,16 +253,16 @@
     <tableColumn id="9" xr3:uid="{E03BC54A-420E-4678-B5AE-9B85B715E6BF}" name="Parameter [data processing software]" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{5C816B2C-913C-4CD6-A90B-FE4C88D10A39}" name="Term Source REF (MS:1001457)" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{3DB29BD0-5556-49A4-89BB-67094991454D}" name="Term Accession Number (MS:1001457)" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{48DC0117-DF25-4E19-95D4-4EDA460F973E}" name="Sample Name"/>
+    <tableColumn id="2" xr3:uid="{48DC0117-DF25-4E19-95D4-4EDA460F973E}" name="Output [Derived Data File]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -300,7 +300,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -406,7 +406,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,14 +560,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -575,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -583,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -599,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -607,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -615,12 +615,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -628,62 +628,62 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -699,159 +699,159 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7265625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.81640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37.81640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7265625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="37.81640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="K2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
         <v>38</v>
       </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="K7" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduce complexity of querymodel testfiles
</commit_message>
<xml_diff>
--- a/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
+++ b/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MSEval_Cold/isa.assay.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E45E72-58B5-4CBD-AA47-1B6EB63DD811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFCF446-912F-4076-8F6E-F00AA48DB9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_assay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>ASSAY</t>
   </si>
@@ -99,15 +99,6 @@
     <t>Assay Person Roles Term Source REF</t>
   </si>
   <si>
-    <t>Parameter [acquisition software]</t>
-  </si>
-  <si>
-    <t>Term Source REF (MS:1001455)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (MS:1001455)</t>
-  </si>
-  <si>
     <t>Parameter [analysis software]</t>
   </si>
   <si>
@@ -115,15 +106,6 @@
   </si>
   <si>
     <t>Term Accession Number (MS:1001456)</t>
-  </si>
-  <si>
-    <t>Parameter [data processing software]</t>
-  </si>
-  <si>
-    <t>Term Source REF (MS:1001457)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (MS:1001457)</t>
   </si>
   <si>
     <t>MSFragger</t>
@@ -198,25 +180,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -240,19 +204,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}" name="annotationTableNiceZebra52" displayName="annotationTableNiceZebra52" ref="A1:K7" totalsRowShown="0">
-  <autoFilter ref="A1:K7" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}" name="annotationTableNiceZebra52" displayName="annotationTableNiceZebra52" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{13B97CD7-72BE-446E-AD79-C67D4619456E}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{35BBF576-4739-4AFC-8D38-3FE476BCD5E1}" name="Input [Raw Data File]"/>
-    <tableColumn id="3" xr3:uid="{252EA98B-77DC-4AB6-BE58-C1B81480FE69}" name="Parameter [acquisition software]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{283FEE7D-D234-44B9-9AD8-16CD15CAC244}" name="Term Source REF (MS:1001455)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{B489FA80-D06A-4FA4-B75B-39F1B7AB9163}" name="Term Accession Number (MS:1001455)" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{708394B2-E3E8-4462-8AB1-948FFE5214A9}" name="Parameter [analysis software]" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{957189FE-7B45-47D0-BEF5-0E19D24D11D8}" name="Term Source REF (MS:1001456)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{ED6D8137-1030-4307-BA4A-D10219B9283B}" name="Term Accession Number (MS:1001456)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{E03BC54A-420E-4678-B5AE-9B85B715E6BF}" name="Parameter [data processing software]" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{5C816B2C-913C-4CD6-A90B-FE4C88D10A39}" name="Term Source REF (MS:1001457)" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{3DB29BD0-5556-49A4-89BB-67094991454D}" name="Term Accession Number (MS:1001457)" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{708394B2-E3E8-4462-8AB1-948FFE5214A9}" name="Parameter [analysis software]" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{957189FE-7B45-47D0-BEF5-0E19D24D11D8}" name="Term Source REF (MS:1001456)" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{ED6D8137-1030-4307-BA4A-D10219B9283B}" name="Term Accession Number (MS:1001456)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{48DC0117-DF25-4E19-95D4-4EDA460F973E}" name="Output [Derived Data File]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -560,14 +518,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -575,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -583,7 +541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -591,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -599,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -607,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -615,12 +573,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -628,62 +586,62 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -696,30 +654,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7381F0D-B8E0-4BFA-8154-D3DBCE3970D1}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -731,127 +683,109 @@
         <v>29</v>
       </c>
       <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>44</v>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>44</v>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>